<commit_message>
added more bv benchmarks
</commit_message>
<xml_diff>
--- a/mpath/src/data/tokyo_zulehner.xlsx
+++ b/mpath/src/data/tokyo_zulehner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SuhasVittal/Documents/programming/quantum_computing/mpath/src/data/sabre_initial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SuhasVittal/Documents/programming/quantum_computing/mpath/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8122C2F8-EA02-3D42-95B8-CCFD9BB7A9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C558CD4-B1E8-6D48-8B32-1BF62E9779BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="28420" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7100" yWindow="260" windowWidth="28420" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tokyo_zulehner" sheetId="1" r:id="rId1"/>
@@ -1223,7 +1223,7 @@
   <dimension ref="A1:O96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>